<commit_message>
modificando el formato de la hora
</commit_message>
<xml_diff>
--- a/static/download/admin/Reporte Detallado de Ventas.xlsx
+++ b/static/download/admin/Reporte Detallado de Ventas.xlsx
@@ -14,18 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="34">
   <si>
     <t>ICT Consulting</t>
   </si>
   <si>
-    <t>Fecha: 2014-11-19</t>
+    <t>Fecha: 2014-11-20</t>
   </si>
   <si>
     <t>REPORTE DE VENTAS</t>
   </si>
   <si>
-    <t>DEL DIA 2014-11-19 0:00:00 AL DIA 2014-11-19 23:59:59</t>
+    <t>DEL DIA 2014-11-20 0:00:00 AL DIA 2014-11-20 23:59:59</t>
   </si>
   <si>
     <t>Ticket</t>
@@ -106,7 +106,16 @@
     <t>C 200.0</t>
   </si>
   <si>
-    <t>3</t>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
   </si>
 </sst>
 </file>
@@ -314,7 +323,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Reporte de ventas del dia" displayName="Reporte de ventas del dia" ref="B10:H70" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Reporte de ventas del dia" displayName="Reporte de ventas del dia" ref="B10:H91" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="7">
     <tableColumn id="1" name="Column1" dataDxfId="0"/>
     <tableColumn id="2" name="Column2" dataDxfId="0"/>
@@ -613,7 +622,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A4:AA70"/>
+  <dimension ref="A4:AA91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -733,32 +742,32 @@
     </row>
     <row r="11" spans="1:27">
       <c r="B11" s="3">
-        <v>1909</v>
+        <v>2261</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D11" s="4">
-        <v>41962.3568518519</v>
+        <v>41963.3763310185</v>
       </c>
       <c r="E11" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F11" s="3">
         <v>1</v>
       </c>
       <c r="G11" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H11" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3">
         <v>1</v>
       </c>
       <c r="K11" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
@@ -779,44 +788,48 @@
     </row>
     <row r="12" spans="1:27">
       <c r="B12" s="3">
-        <v>1910</v>
+        <v>2262</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D12" s="4">
-        <v>41962.3569097222</v>
+        <v>41963.3765509259</v>
       </c>
       <c r="E12" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F12" s="3">
         <v>1</v>
       </c>
       <c r="G12" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H12" s="5">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="I12" s="3"/>
-      <c r="J12" s="3">
-        <v>1</v>
-      </c>
-      <c r="K12" s="3">
-        <v>1</v>
-      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
+      <c r="N12" s="3">
+        <v>1</v>
+      </c>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
       <c r="R12" s="3"/>
       <c r="S12" s="3"/>
-      <c r="T12" s="3"/>
-      <c r="U12" s="3"/>
-      <c r="V12" s="3"/>
+      <c r="T12" s="3">
+        <v>1</v>
+      </c>
+      <c r="U12" s="3">
+        <v>2</v>
+      </c>
+      <c r="V12" s="3">
+        <v>2</v>
+      </c>
       <c r="W12" s="3"/>
       <c r="X12" s="3"/>
       <c r="Y12" s="3"/>
@@ -825,13 +838,13 @@
     </row>
     <row r="13" spans="1:27">
       <c r="B13" s="3">
-        <v>1911</v>
+        <v>2263</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D13" s="4">
-        <v>41962.3569791667</v>
+        <v>41963.3775</v>
       </c>
       <c r="E13" s="5">
         <v>3</v>
@@ -843,24 +856,26 @@
         <v>3</v>
       </c>
       <c r="H13" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I13" s="3"/>
-      <c r="J13" s="3">
-        <v>1</v>
-      </c>
-      <c r="K13" s="3">
-        <v>1</v>
-      </c>
-      <c r="L13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3">
+        <v>1</v>
+      </c>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
-      <c r="S13" s="3"/>
-      <c r="T13" s="3"/>
+      <c r="S13" s="3">
+        <v>2</v>
+      </c>
+      <c r="T13" s="3">
+        <v>1</v>
+      </c>
       <c r="U13" s="3"/>
       <c r="V13" s="3"/>
       <c r="W13" s="3"/>
@@ -871,13 +886,13 @@
     </row>
     <row r="14" spans="1:27">
       <c r="B14" s="3">
-        <v>1912</v>
+        <v>2264</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D14" s="4">
-        <v>41962.3571180556</v>
+        <v>41963.3776967593</v>
       </c>
       <c r="E14" s="5">
         <v>3</v>
@@ -889,29 +904,25 @@
         <v>3</v>
       </c>
       <c r="H14" s="5">
-        <v>3.5</v>
-      </c>
-      <c r="I14" s="3">
-        <v>1</v>
-      </c>
-      <c r="J14" s="3">
-        <v>1</v>
-      </c>
-      <c r="K14" s="3">
-        <v>1</v>
-      </c>
-      <c r="L14" s="3"/>
+        <v>5</v>
+      </c>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3">
+        <v>1</v>
+      </c>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
       <c r="R14" s="3"/>
-      <c r="S14" s="3">
-        <v>1</v>
-      </c>
+      <c r="S14" s="3"/>
       <c r="T14" s="3"/>
-      <c r="U14" s="3"/>
+      <c r="U14" s="3">
+        <v>1</v>
+      </c>
       <c r="V14" s="3"/>
       <c r="W14" s="3"/>
       <c r="X14" s="3"/>
@@ -921,13 +932,13 @@
     </row>
     <row r="15" spans="1:27">
       <c r="B15" s="3">
-        <v>1913</v>
+        <v>2265</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D15" s="4">
-        <v>41962.3795833333</v>
+        <v>41963.3777893518</v>
       </c>
       <c r="E15" s="5">
         <v>3</v>
@@ -939,12 +950,14 @@
         <v>3</v>
       </c>
       <c r="H15" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
+      <c r="J15" s="3">
+        <v>1</v>
+      </c>
       <c r="K15" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
@@ -953,9 +966,7 @@
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
-      <c r="S15" s="3">
-        <v>2</v>
-      </c>
+      <c r="S15" s="3"/>
       <c r="T15" s="3"/>
       <c r="U15" s="3"/>
       <c r="V15" s="3"/>
@@ -967,13 +978,13 @@
     </row>
     <row r="16" spans="1:27">
       <c r="B16" s="3">
-        <v>1914</v>
+        <v>2266</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D16" s="4">
-        <v>41962.3797222222</v>
+        <v>41963.3778587963</v>
       </c>
       <c r="E16" s="5">
         <v>3</v>
@@ -987,10 +998,10 @@
       <c r="H16" s="5">
         <v>3</v>
       </c>
-      <c r="I16" s="3">
-        <v>2</v>
-      </c>
-      <c r="J16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3">
+        <v>1</v>
+      </c>
       <c r="K16" s="3">
         <v>1</v>
       </c>
@@ -1013,13 +1024,13 @@
     </row>
     <row r="17" spans="2:27">
       <c r="B17" s="3">
-        <v>2203</v>
+        <v>2267</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D17" s="4">
-        <v>41962.4640393518</v>
+        <v>41963.3779166667</v>
       </c>
       <c r="E17" s="5">
         <v>3</v>
@@ -1031,31 +1042,27 @@
         <v>3</v>
       </c>
       <c r="H17" s="5">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
+      <c r="J17" s="3">
+        <v>1</v>
+      </c>
+      <c r="K17" s="3">
+        <v>1</v>
+      </c>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
-      <c r="N17" s="3">
-        <v>1</v>
-      </c>
+      <c r="N17" s="3"/>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
       <c r="R17" s="3"/>
       <c r="S17" s="3"/>
-      <c r="T17" s="3">
-        <v>2</v>
-      </c>
+      <c r="T17" s="3"/>
       <c r="U17" s="3"/>
-      <c r="V17" s="3">
-        <v>1</v>
-      </c>
-      <c r="W17" s="3">
-        <v>1</v>
-      </c>
+      <c r="V17" s="3"/>
+      <c r="W17" s="3"/>
       <c r="X17" s="3"/>
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
@@ -1063,13 +1070,13 @@
     </row>
     <row r="18" spans="2:27">
       <c r="B18" s="3">
-        <v>2204</v>
+        <v>2268</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D18" s="4">
-        <v>41962.4642824074</v>
+        <v>41963.3782986111</v>
       </c>
       <c r="E18" s="5">
         <v>3</v>
@@ -1081,31 +1088,31 @@
         <v>3</v>
       </c>
       <c r="H18" s="5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
-      <c r="M18" s="3">
-        <v>1</v>
-      </c>
-      <c r="N18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3">
+        <v>1</v>
+      </c>
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
       <c r="R18" s="3"/>
       <c r="S18" s="3">
-        <v>2</v>
-      </c>
-      <c r="T18" s="3">
-        <v>1</v>
-      </c>
-      <c r="U18" s="3"/>
-      <c r="V18" s="3">
-        <v>1</v>
-      </c>
-      <c r="W18" s="3"/>
+        <v>6</v>
+      </c>
+      <c r="T18" s="3"/>
+      <c r="U18" s="3">
+        <v>2</v>
+      </c>
+      <c r="V18" s="3"/>
+      <c r="W18" s="3">
+        <v>1</v>
+      </c>
       <c r="X18" s="3"/>
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
@@ -1113,13 +1120,13 @@
     </row>
     <row r="19" spans="2:27">
       <c r="B19" s="3">
-        <v>2205</v>
+        <v>2269</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D19" s="4">
-        <v>41962.464375</v>
+        <v>41963.3784259259</v>
       </c>
       <c r="E19" s="5">
         <v>3</v>
@@ -1131,14 +1138,16 @@
         <v>3</v>
       </c>
       <c r="H19" s="5">
-        <v>5</v>
-      </c>
-      <c r="I19" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="I19" s="3">
+        <v>2</v>
+      </c>
       <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3">
-        <v>1</v>
-      </c>
+      <c r="K19" s="3">
+        <v>1</v>
+      </c>
+      <c r="L19" s="3"/>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
@@ -1157,13 +1166,13 @@
     </row>
     <row r="20" spans="2:27">
       <c r="B20" s="3">
-        <v>2206</v>
+        <v>2270</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D20" s="4">
-        <v>41962.4644212963</v>
+        <v>41963.3784490741</v>
       </c>
       <c r="E20" s="5">
         <v>3</v>
@@ -1175,26 +1184,28 @@
         <v>3</v>
       </c>
       <c r="H20" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
-      <c r="L20" s="3">
-        <v>1</v>
-      </c>
-      <c r="M20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3">
+        <v>1</v>
+      </c>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
       <c r="R20" s="3"/>
       <c r="S20" s="3"/>
-      <c r="T20" s="3">
-        <v>2</v>
-      </c>
-      <c r="U20" s="3"/>
-      <c r="V20" s="3"/>
+      <c r="T20" s="3"/>
+      <c r="U20" s="3">
+        <v>1</v>
+      </c>
+      <c r="V20" s="3">
+        <v>1</v>
+      </c>
       <c r="W20" s="3"/>
       <c r="X20" s="3"/>
       <c r="Y20" s="3"/>
@@ -1203,13 +1214,13 @@
     </row>
     <row r="21" spans="2:27">
       <c r="B21" s="3">
-        <v>2207</v>
+        <v>2271</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D21" s="4">
-        <v>41962.4644907407</v>
+        <v>41963.3785300926</v>
       </c>
       <c r="E21" s="5">
         <v>3</v>
@@ -1223,10 +1234,10 @@
       <c r="H21" s="5">
         <v>3</v>
       </c>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3">
-        <v>1</v>
-      </c>
+      <c r="I21" s="3">
+        <v>2</v>
+      </c>
+      <c r="J21" s="3"/>
       <c r="K21" s="3">
         <v>1</v>
       </c>
@@ -1249,13 +1260,13 @@
     </row>
     <row r="22" spans="2:27">
       <c r="B22" s="3">
-        <v>2208</v>
+        <v>2272</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D22" s="4">
-        <v>41962.4650925926</v>
+        <v>41963.3786342593</v>
       </c>
       <c r="E22" s="5">
         <v>3</v>
@@ -1272,10 +1283,10 @@
       <c r="I22" s="3">
         <v>2</v>
       </c>
-      <c r="J22" s="3">
-        <v>2</v>
-      </c>
-      <c r="K22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3">
+        <v>1</v>
+      </c>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
@@ -1295,13 +1306,13 @@
     </row>
     <row r="23" spans="2:27">
       <c r="B23" s="3">
-        <v>2209</v>
+        <v>2273</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D23" s="4">
-        <v>41962.4653240741</v>
+        <v>41963.3786689815</v>
       </c>
       <c r="E23" s="5">
         <v>3</v>
@@ -1313,25 +1324,25 @@
         <v>3</v>
       </c>
       <c r="H23" s="5">
-        <v>51</v>
+        <v>5</v>
       </c>
       <c r="I23" s="3"/>
-      <c r="J23" s="3">
-        <v>1</v>
-      </c>
+      <c r="J23" s="3"/>
       <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
+      <c r="L23" s="3">
+        <v>1</v>
+      </c>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
-      <c r="O23" s="3">
-        <v>1</v>
-      </c>
+      <c r="O23" s="3"/>
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
       <c r="R23" s="3"/>
       <c r="S23" s="3"/>
       <c r="T23" s="3"/>
-      <c r="U23" s="3"/>
+      <c r="U23" s="3">
+        <v>1</v>
+      </c>
       <c r="V23" s="3"/>
       <c r="W23" s="3"/>
       <c r="X23" s="3"/>
@@ -1341,13 +1352,13 @@
     </row>
     <row r="24" spans="2:27">
       <c r="B24" s="3">
-        <v>2210</v>
+        <v>2274</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D24" s="4">
-        <v>41962.4656944444</v>
+        <v>41963.3787615741</v>
       </c>
       <c r="E24" s="5">
         <v>3</v>
@@ -1361,11 +1372,13 @@
       <c r="H24" s="5">
         <v>3</v>
       </c>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3">
-        <v>3</v>
-      </c>
-      <c r="K24" s="3"/>
+      <c r="I24" s="3">
+        <v>2</v>
+      </c>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3">
+        <v>1</v>
+      </c>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
@@ -1385,13 +1398,13 @@
     </row>
     <row r="25" spans="2:27">
       <c r="B25" s="3">
-        <v>2211</v>
+        <v>2275</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D25" s="4">
-        <v>41962.4657407407</v>
+        <v>41963.378900463</v>
       </c>
       <c r="E25" s="5">
         <v>3</v>
@@ -1403,41 +1416,49 @@
         <v>3</v>
       </c>
       <c r="H25" s="5">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="I25" s="3"/>
-      <c r="J25" s="3">
-        <v>1</v>
-      </c>
-      <c r="K25" s="3">
-        <v>1</v>
-      </c>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
-      <c r="P25" s="3"/>
+      <c r="P25" s="3">
+        <v>1</v>
+      </c>
       <c r="Q25" s="3"/>
       <c r="R25" s="3"/>
-      <c r="S25" s="3"/>
-      <c r="T25" s="3"/>
+      <c r="S25" s="3">
+        <v>2</v>
+      </c>
+      <c r="T25" s="3">
+        <v>1</v>
+      </c>
       <c r="U25" s="3"/>
-      <c r="V25" s="3"/>
+      <c r="V25" s="3">
+        <v>1</v>
+      </c>
       <c r="W25" s="3"/>
-      <c r="X25" s="3"/>
-      <c r="Y25" s="3"/>
+      <c r="X25" s="3">
+        <v>2</v>
+      </c>
+      <c r="Y25" s="3">
+        <v>1</v>
+      </c>
       <c r="Z25" s="3"/>
       <c r="AA25" s="3"/>
     </row>
     <row r="26" spans="2:27">
       <c r="B26" s="3">
-        <v>2212</v>
+        <v>2276</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D26" s="4">
-        <v>41962.4658796296</v>
+        <v>41963.3793518519</v>
       </c>
       <c r="E26" s="5">
         <v>3</v>
@@ -1477,13 +1498,13 @@
     </row>
     <row r="27" spans="2:27">
       <c r="B27" s="3">
-        <v>2213</v>
+        <v>2277</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D27" s="4">
-        <v>41962.4660069444</v>
+        <v>41963.3794212963</v>
       </c>
       <c r="E27" s="5">
         <v>3</v>
@@ -1495,31 +1516,29 @@
         <v>3</v>
       </c>
       <c r="H27" s="5">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
+      <c r="L27" s="3">
+        <v>1</v>
+      </c>
       <c r="M27" s="3"/>
-      <c r="N27" s="3">
-        <v>1</v>
-      </c>
+      <c r="N27" s="3"/>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
       <c r="Q27" s="3"/>
       <c r="R27" s="3"/>
-      <c r="S27" s="3"/>
+      <c r="S27" s="3">
+        <v>2</v>
+      </c>
       <c r="T27" s="3">
-        <v>3</v>
-      </c>
-      <c r="U27" s="3">
-        <v>2</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="U27" s="3"/>
       <c r="V27" s="3"/>
-      <c r="W27" s="3">
-        <v>1</v>
-      </c>
+      <c r="W27" s="3"/>
       <c r="X27" s="3"/>
       <c r="Y27" s="3"/>
       <c r="Z27" s="3"/>
@@ -1527,13 +1546,13 @@
     </row>
     <row r="28" spans="2:27">
       <c r="B28" s="3">
-        <v>2214</v>
+        <v>2278</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D28" s="4">
-        <v>41962.466099537</v>
+        <v>41963.3796064815</v>
       </c>
       <c r="E28" s="5">
         <v>3</v>
@@ -1545,27 +1564,33 @@
         <v>3</v>
       </c>
       <c r="H28" s="5">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="I28" s="3"/>
-      <c r="J28" s="3">
-        <v>1</v>
-      </c>
-      <c r="K28" s="3">
-        <v>1</v>
-      </c>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
+      <c r="N28" s="3">
+        <v>1</v>
+      </c>
       <c r="O28" s="3"/>
       <c r="P28" s="3"/>
       <c r="Q28" s="3"/>
       <c r="R28" s="3"/>
-      <c r="S28" s="3"/>
-      <c r="T28" s="3"/>
+      <c r="S28" s="3">
+        <v>2</v>
+      </c>
+      <c r="T28" s="3">
+        <v>1</v>
+      </c>
       <c r="U28" s="3"/>
-      <c r="V28" s="3"/>
-      <c r="W28" s="3"/>
+      <c r="V28" s="3">
+        <v>1</v>
+      </c>
+      <c r="W28" s="3">
+        <v>1</v>
+      </c>
       <c r="X28" s="3"/>
       <c r="Y28" s="3"/>
       <c r="Z28" s="3"/>
@@ -1573,13 +1598,13 @@
     </row>
     <row r="29" spans="2:27">
       <c r="B29" s="3">
-        <v>2215</v>
+        <v>2279</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D29" s="4">
-        <v>41962.4661805556</v>
+        <v>41963.3797569444</v>
       </c>
       <c r="E29" s="5">
         <v>3</v>
@@ -1591,24 +1616,26 @@
         <v>3</v>
       </c>
       <c r="H29" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I29" s="3"/>
-      <c r="J29" s="3">
-        <v>1</v>
-      </c>
-      <c r="K29" s="3">
-        <v>1</v>
-      </c>
-      <c r="L29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3">
+        <v>1</v>
+      </c>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
       <c r="Q29" s="3"/>
       <c r="R29" s="3"/>
-      <c r="S29" s="3"/>
-      <c r="T29" s="3"/>
+      <c r="S29" s="3">
+        <v>2</v>
+      </c>
+      <c r="T29" s="3">
+        <v>1</v>
+      </c>
       <c r="U29" s="3"/>
       <c r="V29" s="3"/>
       <c r="W29" s="3"/>
@@ -1619,13 +1646,13 @@
     </row>
     <row r="30" spans="2:27">
       <c r="B30" s="3">
-        <v>2216</v>
+        <v>2280</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D30" s="4">
-        <v>41962.4662615741</v>
+        <v>41963.3798958333</v>
       </c>
       <c r="E30" s="5">
         <v>3</v>
@@ -1637,27 +1664,25 @@
         <v>3</v>
       </c>
       <c r="H30" s="5">
-        <v>10</v>
-      </c>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="I30" s="3">
+        <v>2</v>
+      </c>
+      <c r="J30" s="3">
+        <v>2</v>
+      </c>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
-      <c r="M30" s="3">
-        <v>1</v>
-      </c>
+      <c r="M30" s="3"/>
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
       <c r="P30" s="3"/>
       <c r="Q30" s="3"/>
       <c r="R30" s="3"/>
-      <c r="S30" s="3">
-        <v>2</v>
-      </c>
+      <c r="S30" s="3"/>
       <c r="T30" s="3"/>
-      <c r="U30" s="3">
-        <v>3</v>
-      </c>
+      <c r="U30" s="3"/>
       <c r="V30" s="3"/>
       <c r="W30" s="3"/>
       <c r="X30" s="3"/>
@@ -1667,13 +1692,13 @@
     </row>
     <row r="31" spans="2:27">
       <c r="B31" s="3">
-        <v>2217</v>
+        <v>2281</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D31" s="4">
-        <v>41962.4663888889</v>
+        <v>41963.3805671296</v>
       </c>
       <c r="E31" s="5">
         <v>3</v>
@@ -1685,25 +1710,29 @@
         <v>3</v>
       </c>
       <c r="H31" s="5">
-        <v>3</v>
-      </c>
-      <c r="I31" s="3">
-        <v>2</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="I31" s="3"/>
       <c r="J31" s="3"/>
-      <c r="K31" s="3">
-        <v>1</v>
-      </c>
+      <c r="K31" s="3"/>
       <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
+      <c r="M31" s="3">
+        <v>1</v>
+      </c>
       <c r="N31" s="3"/>
       <c r="O31" s="3"/>
       <c r="P31" s="3"/>
       <c r="Q31" s="3"/>
       <c r="R31" s="3"/>
-      <c r="S31" s="3"/>
-      <c r="T31" s="3"/>
-      <c r="U31" s="3"/>
+      <c r="S31" s="3">
+        <v>4</v>
+      </c>
+      <c r="T31" s="3">
+        <v>1</v>
+      </c>
+      <c r="U31" s="3">
+        <v>2</v>
+      </c>
       <c r="V31" s="3"/>
       <c r="W31" s="3"/>
       <c r="X31" s="3"/>
@@ -1713,13 +1742,13 @@
     </row>
     <row r="32" spans="2:27">
       <c r="B32" s="3">
-        <v>2218</v>
+        <v>2282</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D32" s="4">
-        <v>41962.4664467593</v>
+        <v>41963.387025463</v>
       </c>
       <c r="E32" s="5">
         <v>3</v>
@@ -1759,13 +1788,13 @@
     </row>
     <row r="33" spans="2:27">
       <c r="B33" s="3">
-        <v>2219</v>
+        <v>2283</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D33" s="4">
-        <v>41962.4665856482</v>
+        <v>41963.4107291667</v>
       </c>
       <c r="E33" s="5">
         <v>3</v>
@@ -1777,32 +1806,26 @@
         <v>3</v>
       </c>
       <c r="H33" s="5">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
+      <c r="J33" s="3">
+        <v>1</v>
+      </c>
+      <c r="K33" s="3">
+        <v>1</v>
+      </c>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
-      <c r="N33" s="3">
-        <v>1</v>
-      </c>
+      <c r="N33" s="3"/>
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
       <c r="Q33" s="3"/>
       <c r="R33" s="3"/>
-      <c r="S33" s="3">
-        <v>2</v>
-      </c>
-      <c r="T33" s="3">
-        <v>3</v>
-      </c>
-      <c r="U33" s="3">
-        <v>4</v>
-      </c>
-      <c r="V33" s="3">
-        <v>1</v>
-      </c>
+      <c r="S33" s="3"/>
+      <c r="T33" s="3"/>
+      <c r="U33" s="3"/>
+      <c r="V33" s="3"/>
       <c r="W33" s="3"/>
       <c r="X33" s="3"/>
       <c r="Y33" s="3"/>
@@ -1811,13 +1834,13 @@
     </row>
     <row r="34" spans="2:27">
       <c r="B34" s="3">
-        <v>2220</v>
+        <v>2284</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D34" s="4">
-        <v>41962.4666666667</v>
+        <v>41963.4109143519</v>
       </c>
       <c r="E34" s="5">
         <v>3</v>
@@ -1831,13 +1854,11 @@
       <c r="H34" s="5">
         <v>3</v>
       </c>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3">
-        <v>1</v>
-      </c>
-      <c r="K34" s="3">
-        <v>1</v>
-      </c>
+      <c r="I34" s="3">
+        <v>6</v>
+      </c>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
       <c r="N34" s="3"/>
@@ -1857,13 +1878,13 @@
     </row>
     <row r="35" spans="2:27">
       <c r="B35" s="3">
-        <v>2221</v>
+        <v>2285</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D35" s="4">
-        <v>41962.4667361111</v>
+        <v>41963.4111574074</v>
       </c>
       <c r="E35" s="5">
         <v>3</v>
@@ -1875,25 +1896,29 @@
         <v>3</v>
       </c>
       <c r="H35" s="5">
-        <v>3</v>
-      </c>
-      <c r="I35" s="3">
-        <v>2</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="I35" s="3"/>
       <c r="J35" s="3"/>
-      <c r="K35" s="3">
-        <v>1</v>
-      </c>
+      <c r="K35" s="3"/>
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
-      <c r="N35" s="3"/>
+      <c r="N35" s="3">
+        <v>1</v>
+      </c>
       <c r="O35" s="3"/>
       <c r="P35" s="3"/>
       <c r="Q35" s="3"/>
       <c r="R35" s="3"/>
-      <c r="S35" s="3"/>
-      <c r="T35" s="3"/>
-      <c r="U35" s="3"/>
+      <c r="S35" s="3">
+        <v>6</v>
+      </c>
+      <c r="T35" s="3">
+        <v>4</v>
+      </c>
+      <c r="U35" s="3">
+        <v>5</v>
+      </c>
       <c r="V35" s="3"/>
       <c r="W35" s="3"/>
       <c r="X35" s="3"/>
@@ -1903,13 +1928,13 @@
     </row>
     <row r="36" spans="2:27">
       <c r="B36" s="3">
-        <v>2222</v>
+        <v>2286</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D36" s="4">
-        <v>41962.4667824074</v>
+        <v>41963.4113194444</v>
       </c>
       <c r="E36" s="5">
         <v>3</v>
@@ -1949,13 +1974,13 @@
     </row>
     <row r="37" spans="2:27">
       <c r="B37" s="3">
-        <v>2223</v>
+        <v>2287</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D37" s="4">
-        <v>41962.4668171296</v>
+        <v>41963.4113888889</v>
       </c>
       <c r="E37" s="5">
         <v>3</v>
@@ -1995,13 +2020,13 @@
     </row>
     <row r="38" spans="2:27">
       <c r="B38" s="3">
-        <v>2224</v>
+        <v>2288</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D38" s="4">
-        <v>41962.4668518519</v>
+        <v>41963.4114583333</v>
       </c>
       <c r="E38" s="5">
         <v>3</v>
@@ -2013,26 +2038,24 @@
         <v>3</v>
       </c>
       <c r="H38" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
-      <c r="L38" s="3">
-        <v>1</v>
-      </c>
+      <c r="J38" s="3">
+        <v>1</v>
+      </c>
+      <c r="K38" s="3">
+        <v>1</v>
+      </c>
+      <c r="L38" s="3"/>
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
       <c r="O38" s="3"/>
       <c r="P38" s="3"/>
       <c r="Q38" s="3"/>
       <c r="R38" s="3"/>
-      <c r="S38" s="3">
-        <v>2</v>
-      </c>
-      <c r="T38" s="3">
-        <v>1</v>
-      </c>
+      <c r="S38" s="3"/>
+      <c r="T38" s="3"/>
       <c r="U38" s="3"/>
       <c r="V38" s="3"/>
       <c r="W38" s="3"/>
@@ -2043,13 +2066,13 @@
     </row>
     <row r="39" spans="2:27">
       <c r="B39" s="3">
-        <v>2225</v>
+        <v>2289</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D39" s="4">
-        <v>41962.4669444444</v>
+        <v>41963.4115393519</v>
       </c>
       <c r="E39" s="5">
         <v>3</v>
@@ -2063,10 +2086,10 @@
       <c r="H39" s="5">
         <v>3</v>
       </c>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3">
-        <v>1</v>
-      </c>
+      <c r="I39" s="3">
+        <v>2</v>
+      </c>
+      <c r="J39" s="3"/>
       <c r="K39" s="3">
         <v>1</v>
       </c>
@@ -2089,13 +2112,13 @@
     </row>
     <row r="40" spans="2:27">
       <c r="B40" s="3">
-        <v>2226</v>
+        <v>2290</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D40" s="4">
-        <v>41962.4671180556</v>
+        <v>41963.4116087963</v>
       </c>
       <c r="E40" s="5">
         <v>3</v>
@@ -2107,45 +2130,41 @@
         <v>3</v>
       </c>
       <c r="H40" s="5">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-      <c r="K40" s="3"/>
+      <c r="J40" s="3">
+        <v>1</v>
+      </c>
+      <c r="K40" s="3">
+        <v>1</v>
+      </c>
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
       <c r="N40" s="3"/>
-      <c r="O40" s="3">
-        <v>1</v>
-      </c>
+      <c r="O40" s="3"/>
       <c r="P40" s="3"/>
       <c r="Q40" s="3"/>
       <c r="R40" s="3"/>
       <c r="S40" s="3"/>
-      <c r="T40" s="3">
-        <v>2</v>
-      </c>
-      <c r="U40" s="3">
-        <v>2</v>
-      </c>
+      <c r="T40" s="3"/>
+      <c r="U40" s="3"/>
       <c r="V40" s="3"/>
       <c r="W40" s="3"/>
-      <c r="X40" s="3">
-        <v>2</v>
-      </c>
+      <c r="X40" s="3"/>
       <c r="Y40" s="3"/>
       <c r="Z40" s="3"/>
       <c r="AA40" s="3"/>
     </row>
     <row r="41" spans="2:27">
       <c r="B41" s="3">
-        <v>2227</v>
+        <v>2291</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D41" s="4">
-        <v>41962.4674421296</v>
+        <v>41963.4117939815</v>
       </c>
       <c r="E41" s="5">
         <v>3</v>
@@ -2159,11 +2178,11 @@
       <c r="H41" s="5">
         <v>3</v>
       </c>
-      <c r="I41" s="3"/>
+      <c r="I41" s="3">
+        <v>6</v>
+      </c>
       <c r="J41" s="3"/>
-      <c r="K41" s="3">
-        <v>1</v>
-      </c>
+      <c r="K41" s="3"/>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
@@ -2183,13 +2202,13 @@
     </row>
     <row r="42" spans="2:27">
       <c r="B42" s="3">
-        <v>2228</v>
+        <v>2292</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D42" s="4">
-        <v>41962.4675694444</v>
+        <v>41963.4137847222</v>
       </c>
       <c r="E42" s="5">
         <v>3</v>
@@ -2201,41 +2220,47 @@
         <v>3</v>
       </c>
       <c r="H42" s="5">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="I42" s="3"/>
-      <c r="J42" s="3">
-        <v>1</v>
-      </c>
-      <c r="K42" s="3">
-        <v>1</v>
-      </c>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
       <c r="N42" s="3"/>
-      <c r="O42" s="3"/>
+      <c r="O42" s="3">
+        <v>1</v>
+      </c>
       <c r="P42" s="3"/>
       <c r="Q42" s="3"/>
       <c r="R42" s="3"/>
-      <c r="S42" s="3"/>
-      <c r="T42" s="3"/>
-      <c r="U42" s="3"/>
+      <c r="S42" s="3">
+        <v>2</v>
+      </c>
+      <c r="T42" s="3">
+        <v>2</v>
+      </c>
+      <c r="U42" s="3">
+        <v>2</v>
+      </c>
       <c r="V42" s="3"/>
       <c r="W42" s="3"/>
-      <c r="X42" s="3"/>
+      <c r="X42" s="3">
+        <v>2</v>
+      </c>
       <c r="Y42" s="3"/>
       <c r="Z42" s="3"/>
       <c r="AA42" s="3"/>
     </row>
     <row r="43" spans="2:27">
       <c r="B43" s="3">
-        <v>2229</v>
+        <v>2293</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D43" s="4">
-        <v>41962.4680671296</v>
+        <v>41963.4141435185</v>
       </c>
       <c r="E43" s="5">
         <v>3</v>
@@ -2247,26 +2272,32 @@
         <v>3</v>
       </c>
       <c r="H43" s="5">
-        <v>3</v>
-      </c>
-      <c r="I43" s="3">
-        <v>4</v>
-      </c>
-      <c r="J43" s="3">
-        <v>1</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
-      <c r="N43" s="3"/>
+      <c r="N43" s="3">
+        <v>1</v>
+      </c>
       <c r="O43" s="3"/>
       <c r="P43" s="3"/>
       <c r="Q43" s="3"/>
       <c r="R43" s="3"/>
-      <c r="S43" s="3"/>
-      <c r="T43" s="3"/>
-      <c r="U43" s="3"/>
-      <c r="V43" s="3"/>
+      <c r="S43" s="3">
+        <v>4</v>
+      </c>
+      <c r="T43" s="3">
+        <v>1</v>
+      </c>
+      <c r="U43" s="3">
+        <v>2</v>
+      </c>
+      <c r="V43" s="3">
+        <v>2</v>
+      </c>
       <c r="W43" s="3"/>
       <c r="X43" s="3"/>
       <c r="Y43" s="3"/>
@@ -2275,13 +2306,13 @@
     </row>
     <row r="44" spans="2:27">
       <c r="B44" s="3">
-        <v>2230</v>
+        <v>2294</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D44" s="4">
-        <v>41962.4682638889</v>
+        <v>41963.4143171296</v>
       </c>
       <c r="E44" s="5">
         <v>3</v>
@@ -2307,14 +2338,12 @@
       <c r="P44" s="3"/>
       <c r="Q44" s="3"/>
       <c r="R44" s="3"/>
-      <c r="S44" s="3">
-        <v>2</v>
-      </c>
+      <c r="S44" s="3"/>
       <c r="T44" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U44" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V44" s="3"/>
       <c r="W44" s="3">
@@ -2327,13 +2356,13 @@
     </row>
     <row r="45" spans="2:27">
       <c r="B45" s="3">
-        <v>2231</v>
+        <v>2295</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D45" s="4">
-        <v>41962.4684953704</v>
+        <v>41963.4143981481</v>
       </c>
       <c r="E45" s="5">
         <v>3</v>
@@ -2345,26 +2374,30 @@
         <v>3</v>
       </c>
       <c r="H45" s="5">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="I45" s="3"/>
-      <c r="J45" s="3">
-        <v>1</v>
-      </c>
-      <c r="K45" s="3">
-        <v>1</v>
-      </c>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
       <c r="L45" s="3"/>
-      <c r="M45" s="3"/>
+      <c r="M45" s="3">
+        <v>1</v>
+      </c>
       <c r="N45" s="3"/>
       <c r="O45" s="3"/>
       <c r="P45" s="3"/>
       <c r="Q45" s="3"/>
       <c r="R45" s="3"/>
-      <c r="S45" s="3"/>
-      <c r="T45" s="3"/>
+      <c r="S45" s="3">
+        <v>2</v>
+      </c>
+      <c r="T45" s="3">
+        <v>1</v>
+      </c>
       <c r="U45" s="3"/>
-      <c r="V45" s="3"/>
+      <c r="V45" s="3">
+        <v>1</v>
+      </c>
       <c r="W45" s="3"/>
       <c r="X45" s="3"/>
       <c r="Y45" s="3"/>
@@ -2373,13 +2406,13 @@
     </row>
     <row r="46" spans="2:27">
       <c r="B46" s="3">
-        <v>2232</v>
+        <v>2296</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D46" s="4">
-        <v>41962.4685648148</v>
+        <v>41963.4144560185</v>
       </c>
       <c r="E46" s="5">
         <v>3</v>
@@ -2391,26 +2424,24 @@
         <v>3</v>
       </c>
       <c r="H46" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
       <c r="K46" s="3"/>
-      <c r="L46" s="3"/>
-      <c r="M46" s="3">
-        <v>1</v>
-      </c>
+      <c r="L46" s="3">
+        <v>1</v>
+      </c>
+      <c r="M46" s="3"/>
       <c r="N46" s="3"/>
       <c r="O46" s="3"/>
       <c r="P46" s="3"/>
       <c r="Q46" s="3"/>
       <c r="R46" s="3"/>
       <c r="S46" s="3"/>
-      <c r="T46" s="3">
-        <v>1</v>
-      </c>
+      <c r="T46" s="3"/>
       <c r="U46" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="V46" s="3"/>
       <c r="W46" s="3"/>
@@ -2421,13 +2452,13 @@
     </row>
     <row r="47" spans="2:27">
       <c r="B47" s="3">
-        <v>2233</v>
+        <v>2297</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D47" s="4">
-        <v>41962.4686458333</v>
+        <v>41963.4145138889</v>
       </c>
       <c r="E47" s="5">
         <v>3</v>
@@ -2439,16 +2470,14 @@
         <v>3</v>
       </c>
       <c r="H47" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I47" s="3"/>
-      <c r="J47" s="3">
-        <v>1</v>
-      </c>
-      <c r="K47" s="3">
-        <v>1</v>
-      </c>
-      <c r="L47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3">
+        <v>1</v>
+      </c>
       <c r="M47" s="3"/>
       <c r="N47" s="3"/>
       <c r="O47" s="3"/>
@@ -2457,7 +2486,9 @@
       <c r="R47" s="3"/>
       <c r="S47" s="3"/>
       <c r="T47" s="3"/>
-      <c r="U47" s="3"/>
+      <c r="U47" s="3">
+        <v>1</v>
+      </c>
       <c r="V47" s="3"/>
       <c r="W47" s="3"/>
       <c r="X47" s="3"/>
@@ -2467,13 +2498,13 @@
     </row>
     <row r="48" spans="2:27">
       <c r="B48" s="3">
-        <v>2234</v>
+        <v>2298</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D48" s="4">
-        <v>41962.4687037037</v>
+        <v>41963.4145717593</v>
       </c>
       <c r="E48" s="5">
         <v>3</v>
@@ -2513,13 +2544,13 @@
     </row>
     <row r="49" spans="2:27">
       <c r="B49" s="3">
-        <v>2235</v>
+        <v>2299</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D49" s="4">
-        <v>41962.4687615741</v>
+        <v>41963.4146527778</v>
       </c>
       <c r="E49" s="5">
         <v>3</v>
@@ -2531,14 +2562,12 @@
         <v>3</v>
       </c>
       <c r="H49" s="5">
-        <v>3</v>
-      </c>
-      <c r="I49" s="3">
-        <v>2</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="I49" s="3"/>
       <c r="J49" s="3"/>
       <c r="K49" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
@@ -2548,7 +2577,9 @@
       <c r="Q49" s="3"/>
       <c r="R49" s="3"/>
       <c r="S49" s="3"/>
-      <c r="T49" s="3"/>
+      <c r="T49" s="3">
+        <v>1</v>
+      </c>
       <c r="U49" s="3"/>
       <c r="V49" s="3"/>
       <c r="W49" s="3"/>
@@ -2559,13 +2590,13 @@
     </row>
     <row r="50" spans="2:27">
       <c r="B50" s="3">
-        <v>2236</v>
+        <v>2300</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D50" s="4">
-        <v>41962.4688773148</v>
+        <v>41963.4147337963</v>
       </c>
       <c r="E50" s="5">
         <v>3</v>
@@ -2577,31 +2608,27 @@
         <v>3</v>
       </c>
       <c r="H50" s="5">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="I50" s="3"/>
       <c r="J50" s="3"/>
-      <c r="K50" s="3"/>
+      <c r="K50" s="3">
+        <v>2</v>
+      </c>
       <c r="L50" s="3"/>
       <c r="M50" s="3"/>
-      <c r="N50" s="3">
-        <v>1</v>
-      </c>
+      <c r="N50" s="3"/>
       <c r="O50" s="3"/>
       <c r="P50" s="3"/>
       <c r="Q50" s="3"/>
       <c r="R50" s="3"/>
-      <c r="S50" s="3"/>
-      <c r="T50" s="3">
-        <v>2</v>
-      </c>
+      <c r="S50" s="3">
+        <v>2</v>
+      </c>
+      <c r="T50" s="3"/>
       <c r="U50" s="3"/>
-      <c r="V50" s="3">
-        <v>1</v>
-      </c>
-      <c r="W50" s="3">
-        <v>1</v>
-      </c>
+      <c r="V50" s="3"/>
+      <c r="W50" s="3"/>
       <c r="X50" s="3"/>
       <c r="Y50" s="3"/>
       <c r="Z50" s="3"/>
@@ -2609,13 +2636,13 @@
     </row>
     <row r="51" spans="2:27">
       <c r="B51" s="3">
-        <v>2237</v>
+        <v>2301</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D51" s="4">
-        <v>41962.4690393519</v>
+        <v>41963.414837963</v>
       </c>
       <c r="E51" s="5">
         <v>3</v>
@@ -2627,27 +2654,25 @@
         <v>3</v>
       </c>
       <c r="H51" s="5">
-        <v>10</v>
-      </c>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="I51" s="3">
+        <v>2</v>
+      </c>
+      <c r="J51" s="3">
+        <v>2</v>
+      </c>
       <c r="K51" s="3"/>
       <c r="L51" s="3"/>
-      <c r="M51" s="3">
-        <v>1</v>
-      </c>
+      <c r="M51" s="3"/>
       <c r="N51" s="3"/>
       <c r="O51" s="3"/>
       <c r="P51" s="3"/>
       <c r="Q51" s="3"/>
       <c r="R51" s="3"/>
       <c r="S51" s="3"/>
-      <c r="T51" s="3">
-        <v>5</v>
-      </c>
-      <c r="U51" s="3">
-        <v>1</v>
-      </c>
+      <c r="T51" s="3"/>
+      <c r="U51" s="3"/>
       <c r="V51" s="3"/>
       <c r="W51" s="3"/>
       <c r="X51" s="3"/>
@@ -2657,13 +2682,13 @@
     </row>
     <row r="52" spans="2:27">
       <c r="B52" s="3">
-        <v>2238</v>
+        <v>2302</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D52" s="4">
-        <v>41962.4691203704</v>
+        <v>41963.4149189815</v>
       </c>
       <c r="E52" s="5">
         <v>3</v>
@@ -2675,26 +2700,24 @@
         <v>3</v>
       </c>
       <c r="H52" s="5">
-        <v>5</v>
-      </c>
-      <c r="I52" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="I52" s="3">
+        <v>2</v>
+      </c>
       <c r="J52" s="3"/>
-      <c r="K52" s="3"/>
-      <c r="L52" s="3">
-        <v>1</v>
-      </c>
+      <c r="K52" s="3">
+        <v>1</v>
+      </c>
+      <c r="L52" s="3"/>
       <c r="M52" s="3"/>
       <c r="N52" s="3"/>
       <c r="O52" s="3"/>
       <c r="P52" s="3"/>
       <c r="Q52" s="3"/>
       <c r="R52" s="3"/>
-      <c r="S52" s="3">
-        <v>2</v>
-      </c>
-      <c r="T52" s="3">
-        <v>1</v>
-      </c>
+      <c r="S52" s="3"/>
+      <c r="T52" s="3"/>
       <c r="U52" s="3"/>
       <c r="V52" s="3"/>
       <c r="W52" s="3"/>
@@ -2705,13 +2728,13 @@
     </row>
     <row r="53" spans="2:27">
       <c r="B53" s="3">
-        <v>2239</v>
+        <v>2303</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D53" s="4">
-        <v>41962.4691898148</v>
+        <v>41963.4149652778</v>
       </c>
       <c r="E53" s="5">
         <v>3</v>
@@ -2723,14 +2746,12 @@
         <v>3</v>
       </c>
       <c r="H53" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I53" s="3"/>
-      <c r="J53" s="3">
-        <v>1</v>
-      </c>
+      <c r="J53" s="3"/>
       <c r="K53" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L53" s="3"/>
       <c r="M53" s="3"/>
@@ -2740,7 +2761,9 @@
       <c r="Q53" s="3"/>
       <c r="R53" s="3"/>
       <c r="S53" s="3"/>
-      <c r="T53" s="3"/>
+      <c r="T53" s="3">
+        <v>1</v>
+      </c>
       <c r="U53" s="3"/>
       <c r="V53" s="3"/>
       <c r="W53" s="3"/>
@@ -2751,13 +2774,13 @@
     </row>
     <row r="54" spans="2:27">
       <c r="B54" s="3">
-        <v>2240</v>
+        <v>2304</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D54" s="4">
-        <v>41962.4692939815</v>
+        <v>41963.4151041667</v>
       </c>
       <c r="E54" s="5">
         <v>3</v>
@@ -2797,13 +2820,13 @@
     </row>
     <row r="55" spans="2:27">
       <c r="B55" s="3">
-        <v>2241</v>
+        <v>2305</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D55" s="4">
-        <v>41962.4693402778</v>
+        <v>41963.4152083333</v>
       </c>
       <c r="E55" s="5">
         <v>3</v>
@@ -2843,13 +2866,13 @@
     </row>
     <row r="56" spans="2:27">
       <c r="B56" s="3">
-        <v>2242</v>
+        <v>2306</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D56" s="4">
-        <v>41962.4694097222</v>
+        <v>41963.4152662037</v>
       </c>
       <c r="E56" s="5">
         <v>3</v>
@@ -2861,23 +2884,29 @@
         <v>3</v>
       </c>
       <c r="H56" s="5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I56" s="3"/>
       <c r="J56" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K56" s="3"/>
-      <c r="L56" s="3"/>
+      <c r="L56" s="3">
+        <v>1</v>
+      </c>
       <c r="M56" s="3"/>
       <c r="N56" s="3"/>
       <c r="O56" s="3"/>
       <c r="P56" s="3"/>
       <c r="Q56" s="3"/>
       <c r="R56" s="3"/>
-      <c r="S56" s="3"/>
+      <c r="S56" s="3">
+        <v>2</v>
+      </c>
       <c r="T56" s="3"/>
-      <c r="U56" s="3"/>
+      <c r="U56" s="3">
+        <v>1</v>
+      </c>
       <c r="V56" s="3"/>
       <c r="W56" s="3"/>
       <c r="X56" s="3"/>
@@ -2887,13 +2916,13 @@
     </row>
     <row r="57" spans="2:27">
       <c r="B57" s="3">
-        <v>2243</v>
+        <v>2307</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D57" s="4">
-        <v>41962.469537037</v>
+        <v>41963.4153703704</v>
       </c>
       <c r="E57" s="5">
         <v>3</v>
@@ -2905,47 +2934,41 @@
         <v>3</v>
       </c>
       <c r="H57" s="5">
-        <v>50</v>
-      </c>
-      <c r="I57" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="I57" s="3">
+        <v>2</v>
+      </c>
       <c r="J57" s="3"/>
-      <c r="K57" s="3"/>
+      <c r="K57" s="3">
+        <v>1</v>
+      </c>
       <c r="L57" s="3"/>
       <c r="M57" s="3"/>
       <c r="N57" s="3"/>
-      <c r="O57" s="3">
-        <v>1</v>
-      </c>
+      <c r="O57" s="3"/>
       <c r="P57" s="3"/>
       <c r="Q57" s="3"/>
       <c r="R57" s="3"/>
-      <c r="S57" s="3">
-        <v>2</v>
-      </c>
-      <c r="T57" s="3">
-        <v>1</v>
-      </c>
+      <c r="S57" s="3"/>
+      <c r="T57" s="3"/>
       <c r="U57" s="3"/>
-      <c r="V57" s="3">
-        <v>1</v>
-      </c>
+      <c r="V57" s="3"/>
       <c r="W57" s="3"/>
-      <c r="X57" s="3">
-        <v>2</v>
-      </c>
+      <c r="X57" s="3"/>
       <c r="Y57" s="3"/>
       <c r="Z57" s="3"/>
       <c r="AA57" s="3"/>
     </row>
     <row r="58" spans="2:27">
       <c r="B58" s="3">
-        <v>2244</v>
+        <v>2308</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D58" s="4">
-        <v>41962.4697916667</v>
+        <v>41963.4180324074</v>
       </c>
       <c r="E58" s="5">
         <v>3</v>
@@ -2957,41 +2980,45 @@
         <v>3</v>
       </c>
       <c r="H58" s="5">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="I58" s="3"/>
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
-      <c r="L58" s="3">
-        <v>1</v>
-      </c>
+      <c r="L58" s="3"/>
       <c r="M58" s="3"/>
       <c r="N58" s="3"/>
-      <c r="O58" s="3"/>
+      <c r="O58" s="3">
+        <v>1</v>
+      </c>
       <c r="P58" s="3"/>
       <c r="Q58" s="3"/>
       <c r="R58" s="3"/>
       <c r="S58" s="3"/>
-      <c r="T58" s="3"/>
+      <c r="T58" s="3">
+        <v>3</v>
+      </c>
       <c r="U58" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V58" s="3"/>
       <c r="W58" s="3"/>
-      <c r="X58" s="3"/>
+      <c r="X58" s="3">
+        <v>2</v>
+      </c>
       <c r="Y58" s="3"/>
       <c r="Z58" s="3"/>
       <c r="AA58" s="3"/>
     </row>
     <row r="59" spans="2:27">
       <c r="B59" s="3">
-        <v>2245</v>
+        <v>2309</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D59" s="4">
-        <v>41962.4698726852</v>
+        <v>41963.4183564815</v>
       </c>
       <c r="E59" s="5">
         <v>3</v>
@@ -3003,26 +3030,30 @@
         <v>3</v>
       </c>
       <c r="H59" s="5">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="I59" s="3"/>
-      <c r="J59" s="3">
-        <v>1</v>
-      </c>
-      <c r="K59" s="3">
-        <v>1</v>
-      </c>
+      <c r="J59" s="3"/>
+      <c r="K59" s="3"/>
       <c r="L59" s="3"/>
       <c r="M59" s="3"/>
-      <c r="N59" s="3"/>
+      <c r="N59" s="3">
+        <v>1</v>
+      </c>
       <c r="O59" s="3"/>
       <c r="P59" s="3"/>
       <c r="Q59" s="3"/>
       <c r="R59" s="3"/>
       <c r="S59" s="3"/>
-      <c r="T59" s="3"/>
-      <c r="U59" s="3"/>
-      <c r="V59" s="3"/>
+      <c r="T59" s="3">
+        <v>1</v>
+      </c>
+      <c r="U59" s="3">
+        <v>3</v>
+      </c>
+      <c r="V59" s="3">
+        <v>2</v>
+      </c>
       <c r="W59" s="3"/>
       <c r="X59" s="3"/>
       <c r="Y59" s="3"/>
@@ -3031,13 +3062,13 @@
     </row>
     <row r="60" spans="2:27">
       <c r="B60" s="3">
-        <v>2246</v>
+        <v>2310</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D60" s="4">
-        <v>41962.4699884259</v>
+        <v>41963.4185532407</v>
       </c>
       <c r="E60" s="5">
         <v>3</v>
@@ -3064,16 +3095,16 @@
       <c r="Q60" s="3"/>
       <c r="R60" s="3"/>
       <c r="S60" s="3"/>
-      <c r="T60" s="3">
-        <v>3</v>
-      </c>
+      <c r="T60" s="3"/>
       <c r="U60" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V60" s="3">
-        <v>2</v>
-      </c>
-      <c r="W60" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="W60" s="3">
+        <v>1</v>
+      </c>
       <c r="X60" s="3"/>
       <c r="Y60" s="3"/>
       <c r="Z60" s="3"/>
@@ -3081,13 +3112,13 @@
     </row>
     <row r="61" spans="2:27">
       <c r="B61" s="3">
-        <v>2247</v>
+        <v>2311</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D61" s="4">
-        <v>41962.4701041667</v>
+        <v>41963.4189351852</v>
       </c>
       <c r="E61" s="5">
         <v>3</v>
@@ -3099,41 +3130,45 @@
         <v>3</v>
       </c>
       <c r="H61" s="5">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="I61" s="3"/>
-      <c r="J61" s="3">
-        <v>1</v>
-      </c>
-      <c r="K61" s="3">
-        <v>1</v>
-      </c>
+      <c r="J61" s="3"/>
+      <c r="K61" s="3"/>
       <c r="L61" s="3"/>
       <c r="M61" s="3"/>
       <c r="N61" s="3"/>
-      <c r="O61" s="3"/>
+      <c r="O61" s="3">
+        <v>1</v>
+      </c>
       <c r="P61" s="3"/>
       <c r="Q61" s="3"/>
       <c r="R61" s="3"/>
       <c r="S61" s="3"/>
-      <c r="T61" s="3"/>
+      <c r="T61" s="3">
+        <v>2</v>
+      </c>
       <c r="U61" s="3"/>
-      <c r="V61" s="3"/>
+      <c r="V61" s="3">
+        <v>1</v>
+      </c>
       <c r="W61" s="3"/>
-      <c r="X61" s="3"/>
+      <c r="X61" s="3">
+        <v>2</v>
+      </c>
       <c r="Y61" s="3"/>
       <c r="Z61" s="3"/>
       <c r="AA61" s="3"/>
     </row>
     <row r="62" spans="2:27">
       <c r="B62" s="3">
-        <v>2248</v>
+        <v>2312</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D62" s="4">
-        <v>41962.4701967593</v>
+        <v>41963.4192939815</v>
       </c>
       <c r="E62" s="5">
         <v>3</v>
@@ -3145,26 +3180,32 @@
         <v>3</v>
       </c>
       <c r="H62" s="5">
-        <v>3</v>
-      </c>
-      <c r="I62" s="3">
-        <v>2</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="I62" s="3"/>
       <c r="J62" s="3"/>
-      <c r="K62" s="3">
-        <v>1</v>
-      </c>
+      <c r="K62" s="3"/>
       <c r="L62" s="3"/>
       <c r="M62" s="3"/>
-      <c r="N62" s="3"/>
+      <c r="N62" s="3">
+        <v>1</v>
+      </c>
       <c r="O62" s="3"/>
       <c r="P62" s="3"/>
       <c r="Q62" s="3"/>
       <c r="R62" s="3"/>
-      <c r="S62" s="3"/>
-      <c r="T62" s="3"/>
-      <c r="U62" s="3"/>
-      <c r="V62" s="3"/>
+      <c r="S62" s="3">
+        <v>4</v>
+      </c>
+      <c r="T62" s="3">
+        <v>1</v>
+      </c>
+      <c r="U62" s="3">
+        <v>2</v>
+      </c>
+      <c r="V62" s="3">
+        <v>2</v>
+      </c>
       <c r="W62" s="3"/>
       <c r="X62" s="3"/>
       <c r="Y62" s="3"/>
@@ -3173,13 +3214,13 @@
     </row>
     <row r="63" spans="2:27">
       <c r="B63" s="3">
-        <v>2249</v>
+        <v>2313</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D63" s="4">
-        <v>41962.4702314815</v>
+        <v>41963.4195833333</v>
       </c>
       <c r="E63" s="5">
         <v>3</v>
@@ -3191,26 +3232,32 @@
         <v>3</v>
       </c>
       <c r="H63" s="5">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I63" s="3"/>
       <c r="J63" s="3"/>
       <c r="K63" s="3"/>
-      <c r="L63" s="3">
-        <v>1</v>
-      </c>
+      <c r="L63" s="3"/>
       <c r="M63" s="3"/>
-      <c r="N63" s="3"/>
+      <c r="N63" s="3">
+        <v>1</v>
+      </c>
       <c r="O63" s="3"/>
       <c r="P63" s="3"/>
       <c r="Q63" s="3"/>
       <c r="R63" s="3"/>
-      <c r="S63" s="3"/>
-      <c r="T63" s="3"/>
+      <c r="S63" s="3">
+        <v>2</v>
+      </c>
+      <c r="T63" s="3">
+        <v>3</v>
+      </c>
       <c r="U63" s="3">
-        <v>1</v>
-      </c>
-      <c r="V63" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="V63" s="3">
+        <v>1</v>
+      </c>
       <c r="W63" s="3"/>
       <c r="X63" s="3"/>
       <c r="Y63" s="3"/>
@@ -3219,13 +3266,13 @@
     </row>
     <row r="64" spans="2:27">
       <c r="B64" s="3">
-        <v>2250</v>
+        <v>2314</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D64" s="4">
-        <v>41962.4703125</v>
+        <v>41963.4197106482</v>
       </c>
       <c r="E64" s="5">
         <v>3</v>
@@ -3237,23 +3284,23 @@
         <v>3</v>
       </c>
       <c r="H64" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I64" s="3"/>
-      <c r="J64" s="3">
-        <v>1</v>
-      </c>
-      <c r="K64" s="3">
-        <v>1</v>
-      </c>
-      <c r="L64" s="3"/>
+      <c r="J64" s="3"/>
+      <c r="K64" s="3"/>
+      <c r="L64" s="3">
+        <v>1</v>
+      </c>
       <c r="M64" s="3"/>
       <c r="N64" s="3"/>
       <c r="O64" s="3"/>
       <c r="P64" s="3"/>
       <c r="Q64" s="3"/>
       <c r="R64" s="3"/>
-      <c r="S64" s="3"/>
+      <c r="S64" s="3">
+        <v>4</v>
+      </c>
       <c r="T64" s="3"/>
       <c r="U64" s="3"/>
       <c r="V64" s="3"/>
@@ -3265,13 +3312,13 @@
     </row>
     <row r="65" spans="2:27">
       <c r="B65" s="3">
-        <v>2251</v>
+        <v>2315</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D65" s="4">
-        <v>41962.4703935185</v>
+        <v>41963.4199884259</v>
       </c>
       <c r="E65" s="5">
         <v>3</v>
@@ -3283,15 +3330,15 @@
         <v>3</v>
       </c>
       <c r="H65" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I65" s="3"/>
       <c r="J65" s="3"/>
       <c r="K65" s="3"/>
-      <c r="L65" s="3">
-        <v>1</v>
-      </c>
-      <c r="M65" s="3"/>
+      <c r="L65" s="3"/>
+      <c r="M65" s="3">
+        <v>1</v>
+      </c>
       <c r="N65" s="3"/>
       <c r="O65" s="3"/>
       <c r="P65" s="3"/>
@@ -3301,9 +3348,11 @@
         <v>2</v>
       </c>
       <c r="T65" s="3">
-        <v>1</v>
-      </c>
-      <c r="U65" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="U65" s="3">
+        <v>2</v>
+      </c>
       <c r="V65" s="3"/>
       <c r="W65" s="3"/>
       <c r="X65" s="3"/>
@@ -3313,13 +3362,13 @@
     </row>
     <row r="66" spans="2:27">
       <c r="B66" s="3">
-        <v>2252</v>
+        <v>2316</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D66" s="4">
-        <v>41962.4705208333</v>
+        <v>41963.4201273148</v>
       </c>
       <c r="E66" s="5">
         <v>3</v>
@@ -3331,15 +3380,13 @@
         <v>3</v>
       </c>
       <c r="H66" s="5">
-        <v>3</v>
-      </c>
-      <c r="I66" s="3">
-        <v>2</v>
-      </c>
-      <c r="J66" s="3">
-        <v>2</v>
-      </c>
-      <c r="K66" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="I66" s="3"/>
+      <c r="J66" s="3"/>
+      <c r="K66" s="3">
+        <v>2</v>
+      </c>
       <c r="L66" s="3"/>
       <c r="M66" s="3"/>
       <c r="N66" s="3"/>
@@ -3348,7 +3395,9 @@
       <c r="Q66" s="3"/>
       <c r="R66" s="3"/>
       <c r="S66" s="3"/>
-      <c r="T66" s="3"/>
+      <c r="T66" s="3">
+        <v>1</v>
+      </c>
       <c r="U66" s="3"/>
       <c r="V66" s="3"/>
       <c r="W66" s="3"/>
@@ -3359,13 +3408,13 @@
     </row>
     <row r="67" spans="2:27">
       <c r="B67" s="3">
-        <v>2253</v>
+        <v>2317</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D67" s="4">
-        <v>41962.4708449074</v>
+        <v>41963.4201967593</v>
       </c>
       <c r="E67" s="5">
         <v>3</v>
@@ -3377,16 +3426,16 @@
         <v>3</v>
       </c>
       <c r="H67" s="5">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="I67" s="3"/>
       <c r="J67" s="3"/>
       <c r="K67" s="3"/>
-      <c r="L67" s="3"/>
+      <c r="L67" s="3">
+        <v>1</v>
+      </c>
       <c r="M67" s="3"/>
-      <c r="N67" s="3">
-        <v>1</v>
-      </c>
+      <c r="N67" s="3"/>
       <c r="O67" s="3"/>
       <c r="P67" s="3"/>
       <c r="Q67" s="3"/>
@@ -3398,12 +3447,8 @@
         <v>1</v>
       </c>
       <c r="U67" s="3"/>
-      <c r="V67" s="3">
-        <v>1</v>
-      </c>
-      <c r="W67" s="3">
-        <v>1</v>
-      </c>
+      <c r="V67" s="3"/>
+      <c r="W67" s="3"/>
       <c r="X67" s="3"/>
       <c r="Y67" s="3"/>
       <c r="Z67" s="3"/>
@@ -3411,13 +3456,13 @@
     </row>
     <row r="68" spans="2:27">
       <c r="B68" s="3">
-        <v>2254</v>
+        <v>2318</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D68" s="4">
-        <v>41962.4888310185</v>
+        <v>41963.4202777778</v>
       </c>
       <c r="E68" s="5">
         <v>3</v>
@@ -3429,14 +3474,12 @@
         <v>3</v>
       </c>
       <c r="H68" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I68" s="3"/>
-      <c r="J68" s="3">
-        <v>1</v>
-      </c>
+      <c r="J68" s="3"/>
       <c r="K68" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L68" s="3"/>
       <c r="M68" s="3"/>
@@ -3445,7 +3488,9 @@
       <c r="P68" s="3"/>
       <c r="Q68" s="3"/>
       <c r="R68" s="3"/>
-      <c r="S68" s="3"/>
+      <c r="S68" s="3">
+        <v>2</v>
+      </c>
       <c r="T68" s="3"/>
       <c r="U68" s="3"/>
       <c r="V68" s="3"/>
@@ -3457,13 +3502,13 @@
     </row>
     <row r="69" spans="2:27">
       <c r="B69" s="3">
-        <v>2255</v>
+        <v>2319</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D69" s="4">
-        <v>41962.540162037</v>
+        <v>41963.4203587963</v>
       </c>
       <c r="E69" s="5">
         <v>3</v>
@@ -3475,29 +3520,23 @@
         <v>3</v>
       </c>
       <c r="H69" s="5">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I69" s="3"/>
-      <c r="J69" s="3"/>
+      <c r="J69" s="3">
+        <v>3</v>
+      </c>
       <c r="K69" s="3"/>
       <c r="L69" s="3"/>
-      <c r="M69" s="3">
-        <v>1</v>
-      </c>
+      <c r="M69" s="3"/>
       <c r="N69" s="3"/>
       <c r="O69" s="3"/>
       <c r="P69" s="3"/>
       <c r="Q69" s="3"/>
       <c r="R69" s="3"/>
-      <c r="S69" s="3">
-        <v>2</v>
-      </c>
-      <c r="T69" s="3">
-        <v>2</v>
-      </c>
-      <c r="U69" s="3">
-        <v>2</v>
-      </c>
+      <c r="S69" s="3"/>
+      <c r="T69" s="3"/>
+      <c r="U69" s="3"/>
       <c r="V69" s="3"/>
       <c r="W69" s="3"/>
       <c r="X69" s="3"/>
@@ -3507,13 +3546,13 @@
     </row>
     <row r="70" spans="2:27">
       <c r="B70" s="3">
-        <v>2256</v>
+        <v>2320</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D70" s="4">
-        <v>41962.6522800926</v>
+        <v>41963.4203935185</v>
       </c>
       <c r="E70" s="5">
         <v>3</v>
@@ -3525,24 +3564,26 @@
         <v>3</v>
       </c>
       <c r="H70" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I70" s="3"/>
-      <c r="J70" s="3">
-        <v>1</v>
-      </c>
-      <c r="K70" s="3">
-        <v>1</v>
-      </c>
-      <c r="L70" s="3"/>
+      <c r="J70" s="3"/>
+      <c r="K70" s="3"/>
+      <c r="L70" s="3">
+        <v>1</v>
+      </c>
       <c r="M70" s="3"/>
       <c r="N70" s="3"/>
       <c r="O70" s="3"/>
       <c r="P70" s="3"/>
       <c r="Q70" s="3"/>
       <c r="R70" s="3"/>
-      <c r="S70" s="3"/>
-      <c r="T70" s="3"/>
+      <c r="S70" s="3">
+        <v>2</v>
+      </c>
+      <c r="T70" s="3">
+        <v>1</v>
+      </c>
       <c r="U70" s="3"/>
       <c r="V70" s="3"/>
       <c r="W70" s="3"/>
@@ -3550,6 +3591,968 @@
       <c r="Y70" s="3"/>
       <c r="Z70" s="3"/>
       <c r="AA70" s="3"/>
+    </row>
+    <row r="71" spans="2:27">
+      <c r="B71" s="3">
+        <v>2321</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D71" s="4">
+        <v>41963.4204976852</v>
+      </c>
+      <c r="E71" s="5">
+        <v>3</v>
+      </c>
+      <c r="F71" s="3">
+        <v>1</v>
+      </c>
+      <c r="G71" s="5">
+        <v>3</v>
+      </c>
+      <c r="H71" s="5">
+        <v>3</v>
+      </c>
+      <c r="I71" s="3"/>
+      <c r="J71" s="3">
+        <v>1</v>
+      </c>
+      <c r="K71" s="3">
+        <v>1</v>
+      </c>
+      <c r="L71" s="3"/>
+      <c r="M71" s="3"/>
+      <c r="N71" s="3"/>
+      <c r="O71" s="3"/>
+      <c r="P71" s="3"/>
+      <c r="Q71" s="3"/>
+      <c r="R71" s="3"/>
+      <c r="S71" s="3"/>
+      <c r="T71" s="3"/>
+      <c r="U71" s="3"/>
+      <c r="V71" s="3"/>
+      <c r="W71" s="3"/>
+      <c r="X71" s="3"/>
+      <c r="Y71" s="3"/>
+      <c r="Z71" s="3"/>
+      <c r="AA71" s="3"/>
+    </row>
+    <row r="72" spans="2:27">
+      <c r="B72" s="3">
+        <v>2322</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D72" s="4">
+        <v>41963.4206018519</v>
+      </c>
+      <c r="E72" s="5">
+        <v>3</v>
+      </c>
+      <c r="F72" s="3">
+        <v>1</v>
+      </c>
+      <c r="G72" s="5">
+        <v>3</v>
+      </c>
+      <c r="H72" s="5">
+        <v>4</v>
+      </c>
+      <c r="I72" s="3"/>
+      <c r="J72" s="3"/>
+      <c r="K72" s="3">
+        <v>2</v>
+      </c>
+      <c r="L72" s="3"/>
+      <c r="M72" s="3"/>
+      <c r="N72" s="3"/>
+      <c r="O72" s="3"/>
+      <c r="P72" s="3"/>
+      <c r="Q72" s="3"/>
+      <c r="R72" s="3"/>
+      <c r="S72" s="3"/>
+      <c r="T72" s="3">
+        <v>1</v>
+      </c>
+      <c r="U72" s="3"/>
+      <c r="V72" s="3"/>
+      <c r="W72" s="3"/>
+      <c r="X72" s="3"/>
+      <c r="Y72" s="3"/>
+      <c r="Z72" s="3"/>
+      <c r="AA72" s="3"/>
+    </row>
+    <row r="73" spans="2:27">
+      <c r="B73" s="3">
+        <v>2323</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D73" s="4">
+        <v>41963.4206597222</v>
+      </c>
+      <c r="E73" s="5">
+        <v>3</v>
+      </c>
+      <c r="F73" s="3">
+        <v>1</v>
+      </c>
+      <c r="G73" s="5">
+        <v>3</v>
+      </c>
+      <c r="H73" s="5">
+        <v>5</v>
+      </c>
+      <c r="I73" s="3"/>
+      <c r="J73" s="3"/>
+      <c r="K73" s="3"/>
+      <c r="L73" s="3">
+        <v>1</v>
+      </c>
+      <c r="M73" s="3"/>
+      <c r="N73" s="3"/>
+      <c r="O73" s="3"/>
+      <c r="P73" s="3"/>
+      <c r="Q73" s="3"/>
+      <c r="R73" s="3"/>
+      <c r="S73" s="3">
+        <v>2</v>
+      </c>
+      <c r="T73" s="3">
+        <v>1</v>
+      </c>
+      <c r="U73" s="3"/>
+      <c r="V73" s="3"/>
+      <c r="W73" s="3"/>
+      <c r="X73" s="3"/>
+      <c r="Y73" s="3"/>
+      <c r="Z73" s="3"/>
+      <c r="AA73" s="3"/>
+    </row>
+    <row r="74" spans="2:27">
+      <c r="B74" s="3">
+        <v>2324</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D74" s="4">
+        <v>41963.4207175926</v>
+      </c>
+      <c r="E74" s="5">
+        <v>3</v>
+      </c>
+      <c r="F74" s="3">
+        <v>1</v>
+      </c>
+      <c r="G74" s="5">
+        <v>3</v>
+      </c>
+      <c r="H74" s="5">
+        <v>4</v>
+      </c>
+      <c r="I74" s="3"/>
+      <c r="J74" s="3"/>
+      <c r="K74" s="3">
+        <v>2</v>
+      </c>
+      <c r="L74" s="3"/>
+      <c r="M74" s="3"/>
+      <c r="N74" s="3"/>
+      <c r="O74" s="3"/>
+      <c r="P74" s="3"/>
+      <c r="Q74" s="3"/>
+      <c r="R74" s="3"/>
+      <c r="S74" s="3">
+        <v>2</v>
+      </c>
+      <c r="T74" s="3"/>
+      <c r="U74" s="3"/>
+      <c r="V74" s="3"/>
+      <c r="W74" s="3"/>
+      <c r="X74" s="3"/>
+      <c r="Y74" s="3"/>
+      <c r="Z74" s="3"/>
+      <c r="AA74" s="3"/>
+    </row>
+    <row r="75" spans="2:27">
+      <c r="B75" s="3">
+        <v>2325</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D75" s="4">
+        <v>41963.4208449074</v>
+      </c>
+      <c r="E75" s="5">
+        <v>3</v>
+      </c>
+      <c r="F75" s="3">
+        <v>1</v>
+      </c>
+      <c r="G75" s="5">
+        <v>3</v>
+      </c>
+      <c r="H75" s="5">
+        <v>3</v>
+      </c>
+      <c r="I75" s="3">
+        <v>6</v>
+      </c>
+      <c r="J75" s="3"/>
+      <c r="K75" s="3"/>
+      <c r="L75" s="3"/>
+      <c r="M75" s="3"/>
+      <c r="N75" s="3"/>
+      <c r="O75" s="3"/>
+      <c r="P75" s="3"/>
+      <c r="Q75" s="3"/>
+      <c r="R75" s="3"/>
+      <c r="S75" s="3"/>
+      <c r="T75" s="3"/>
+      <c r="U75" s="3"/>
+      <c r="V75" s="3"/>
+      <c r="W75" s="3"/>
+      <c r="X75" s="3"/>
+      <c r="Y75" s="3"/>
+      <c r="Z75" s="3"/>
+      <c r="AA75" s="3"/>
+    </row>
+    <row r="76" spans="2:27">
+      <c r="B76" s="3">
+        <v>2326</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D76" s="4">
+        <v>41963.4209375</v>
+      </c>
+      <c r="E76" s="5">
+        <v>3</v>
+      </c>
+      <c r="F76" s="3">
+        <v>1</v>
+      </c>
+      <c r="G76" s="5">
+        <v>3</v>
+      </c>
+      <c r="H76" s="5">
+        <v>3</v>
+      </c>
+      <c r="I76" s="3"/>
+      <c r="J76" s="3">
+        <v>1</v>
+      </c>
+      <c r="K76" s="3">
+        <v>1</v>
+      </c>
+      <c r="L76" s="3"/>
+      <c r="M76" s="3"/>
+      <c r="N76" s="3"/>
+      <c r="O76" s="3"/>
+      <c r="P76" s="3"/>
+      <c r="Q76" s="3"/>
+      <c r="R76" s="3"/>
+      <c r="S76" s="3"/>
+      <c r="T76" s="3"/>
+      <c r="U76" s="3"/>
+      <c r="V76" s="3"/>
+      <c r="W76" s="3"/>
+      <c r="X76" s="3"/>
+      <c r="Y76" s="3"/>
+      <c r="Z76" s="3"/>
+      <c r="AA76" s="3"/>
+    </row>
+    <row r="77" spans="2:27">
+      <c r="B77" s="3">
+        <v>2327</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D77" s="4">
+        <v>41963.4209722222</v>
+      </c>
+      <c r="E77" s="5">
+        <v>3</v>
+      </c>
+      <c r="F77" s="3">
+        <v>1</v>
+      </c>
+      <c r="G77" s="5">
+        <v>3</v>
+      </c>
+      <c r="H77" s="5">
+        <v>3</v>
+      </c>
+      <c r="I77" s="3"/>
+      <c r="J77" s="3">
+        <v>1</v>
+      </c>
+      <c r="K77" s="3">
+        <v>1</v>
+      </c>
+      <c r="L77" s="3"/>
+      <c r="M77" s="3"/>
+      <c r="N77" s="3"/>
+      <c r="O77" s="3"/>
+      <c r="P77" s="3"/>
+      <c r="Q77" s="3"/>
+      <c r="R77" s="3"/>
+      <c r="S77" s="3"/>
+      <c r="T77" s="3"/>
+      <c r="U77" s="3"/>
+      <c r="V77" s="3"/>
+      <c r="W77" s="3"/>
+      <c r="X77" s="3"/>
+      <c r="Y77" s="3"/>
+      <c r="Z77" s="3"/>
+      <c r="AA77" s="3"/>
+    </row>
+    <row r="78" spans="2:27">
+      <c r="B78" s="3">
+        <v>2328</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D78" s="4">
+        <v>41963.4210069444</v>
+      </c>
+      <c r="E78" s="5">
+        <v>3</v>
+      </c>
+      <c r="F78" s="3">
+        <v>1</v>
+      </c>
+      <c r="G78" s="5">
+        <v>3</v>
+      </c>
+      <c r="H78" s="5">
+        <v>5</v>
+      </c>
+      <c r="I78" s="3"/>
+      <c r="J78" s="3"/>
+      <c r="K78" s="3"/>
+      <c r="L78" s="3">
+        <v>1</v>
+      </c>
+      <c r="M78" s="3"/>
+      <c r="N78" s="3"/>
+      <c r="O78" s="3"/>
+      <c r="P78" s="3"/>
+      <c r="Q78" s="3"/>
+      <c r="R78" s="3"/>
+      <c r="S78" s="3"/>
+      <c r="T78" s="3"/>
+      <c r="U78" s="3">
+        <v>1</v>
+      </c>
+      <c r="V78" s="3"/>
+      <c r="W78" s="3"/>
+      <c r="X78" s="3"/>
+      <c r="Y78" s="3"/>
+      <c r="Z78" s="3"/>
+      <c r="AA78" s="3"/>
+    </row>
+    <row r="79" spans="2:27">
+      <c r="B79" s="3">
+        <v>2329</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D79" s="4">
+        <v>41963.4211574074</v>
+      </c>
+      <c r="E79" s="5">
+        <v>3</v>
+      </c>
+      <c r="F79" s="3">
+        <v>1</v>
+      </c>
+      <c r="G79" s="5">
+        <v>3</v>
+      </c>
+      <c r="H79" s="5">
+        <v>4</v>
+      </c>
+      <c r="I79" s="3"/>
+      <c r="J79" s="3">
+        <v>2</v>
+      </c>
+      <c r="K79" s="3">
+        <v>1</v>
+      </c>
+      <c r="L79" s="3"/>
+      <c r="M79" s="3"/>
+      <c r="N79" s="3"/>
+      <c r="O79" s="3"/>
+      <c r="P79" s="3"/>
+      <c r="Q79" s="3"/>
+      <c r="R79" s="3"/>
+      <c r="S79" s="3">
+        <v>2</v>
+      </c>
+      <c r="T79" s="3"/>
+      <c r="U79" s="3"/>
+      <c r="V79" s="3"/>
+      <c r="W79" s="3"/>
+      <c r="X79" s="3"/>
+      <c r="Y79" s="3"/>
+      <c r="Z79" s="3"/>
+      <c r="AA79" s="3"/>
+    </row>
+    <row r="80" spans="2:27">
+      <c r="B80" s="3">
+        <v>2330</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D80" s="4">
+        <v>41963.421400463</v>
+      </c>
+      <c r="E80" s="5">
+        <v>3</v>
+      </c>
+      <c r="F80" s="3">
+        <v>1</v>
+      </c>
+      <c r="G80" s="5">
+        <v>3</v>
+      </c>
+      <c r="H80" s="5">
+        <v>3</v>
+      </c>
+      <c r="I80" s="3">
+        <v>6</v>
+      </c>
+      <c r="J80" s="3"/>
+      <c r="K80" s="3"/>
+      <c r="L80" s="3"/>
+      <c r="M80" s="3"/>
+      <c r="N80" s="3"/>
+      <c r="O80" s="3"/>
+      <c r="P80" s="3"/>
+      <c r="Q80" s="3"/>
+      <c r="R80" s="3"/>
+      <c r="S80" s="3"/>
+      <c r="T80" s="3"/>
+      <c r="U80" s="3"/>
+      <c r="V80" s="3"/>
+      <c r="W80" s="3"/>
+      <c r="X80" s="3"/>
+      <c r="Y80" s="3"/>
+      <c r="Z80" s="3"/>
+      <c r="AA80" s="3"/>
+    </row>
+    <row r="81" spans="2:27">
+      <c r="B81" s="3">
+        <v>2331</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D81" s="4">
+        <v>41963.4214467593</v>
+      </c>
+      <c r="E81" s="5">
+        <v>3</v>
+      </c>
+      <c r="F81" s="3">
+        <v>1</v>
+      </c>
+      <c r="G81" s="5">
+        <v>3</v>
+      </c>
+      <c r="H81" s="5">
+        <v>3</v>
+      </c>
+      <c r="I81" s="3"/>
+      <c r="J81" s="3">
+        <v>1</v>
+      </c>
+      <c r="K81" s="3">
+        <v>1</v>
+      </c>
+      <c r="L81" s="3"/>
+      <c r="M81" s="3"/>
+      <c r="N81" s="3"/>
+      <c r="O81" s="3"/>
+      <c r="P81" s="3"/>
+      <c r="Q81" s="3"/>
+      <c r="R81" s="3"/>
+      <c r="S81" s="3"/>
+      <c r="T81" s="3"/>
+      <c r="U81" s="3"/>
+      <c r="V81" s="3"/>
+      <c r="W81" s="3"/>
+      <c r="X81" s="3"/>
+      <c r="Y81" s="3"/>
+      <c r="Z81" s="3"/>
+      <c r="AA81" s="3"/>
+    </row>
+    <row r="82" spans="2:27">
+      <c r="B82" s="3">
+        <v>2332</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D82" s="4">
+        <v>41963.4215046296</v>
+      </c>
+      <c r="E82" s="5">
+        <v>3</v>
+      </c>
+      <c r="F82" s="3">
+        <v>1</v>
+      </c>
+      <c r="G82" s="5">
+        <v>3</v>
+      </c>
+      <c r="H82" s="5">
+        <v>3</v>
+      </c>
+      <c r="I82" s="3"/>
+      <c r="J82" s="3">
+        <v>1</v>
+      </c>
+      <c r="K82" s="3">
+        <v>1</v>
+      </c>
+      <c r="L82" s="3"/>
+      <c r="M82" s="3"/>
+      <c r="N82" s="3"/>
+      <c r="O82" s="3"/>
+      <c r="P82" s="3"/>
+      <c r="Q82" s="3"/>
+      <c r="R82" s="3"/>
+      <c r="S82" s="3"/>
+      <c r="T82" s="3"/>
+      <c r="U82" s="3"/>
+      <c r="V82" s="3"/>
+      <c r="W82" s="3"/>
+      <c r="X82" s="3"/>
+      <c r="Y82" s="3"/>
+      <c r="Z82" s="3"/>
+      <c r="AA82" s="3"/>
+    </row>
+    <row r="83" spans="2:27">
+      <c r="B83" s="3">
+        <v>2333</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D83" s="4">
+        <v>41963.4215740741</v>
+      </c>
+      <c r="E83" s="5">
+        <v>3</v>
+      </c>
+      <c r="F83" s="3">
+        <v>1</v>
+      </c>
+      <c r="G83" s="5">
+        <v>3</v>
+      </c>
+      <c r="H83" s="5">
+        <v>3</v>
+      </c>
+      <c r="I83" s="3">
+        <v>2</v>
+      </c>
+      <c r="J83" s="3">
+        <v>2</v>
+      </c>
+      <c r="K83" s="3"/>
+      <c r="L83" s="3"/>
+      <c r="M83" s="3"/>
+      <c r="N83" s="3"/>
+      <c r="O83" s="3"/>
+      <c r="P83" s="3"/>
+      <c r="Q83" s="3"/>
+      <c r="R83" s="3"/>
+      <c r="S83" s="3"/>
+      <c r="T83" s="3"/>
+      <c r="U83" s="3"/>
+      <c r="V83" s="3"/>
+      <c r="W83" s="3"/>
+      <c r="X83" s="3"/>
+      <c r="Y83" s="3"/>
+      <c r="Z83" s="3"/>
+      <c r="AA83" s="3"/>
+    </row>
+    <row r="84" spans="2:27">
+      <c r="B84" s="3">
+        <v>2334</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D84" s="4">
+        <v>41963.4216087963</v>
+      </c>
+      <c r="E84" s="5">
+        <v>3</v>
+      </c>
+      <c r="F84" s="3">
+        <v>1</v>
+      </c>
+      <c r="G84" s="5">
+        <v>3</v>
+      </c>
+      <c r="H84" s="5">
+        <v>5</v>
+      </c>
+      <c r="I84" s="3"/>
+      <c r="J84" s="3"/>
+      <c r="K84" s="3"/>
+      <c r="L84" s="3">
+        <v>1</v>
+      </c>
+      <c r="M84" s="3"/>
+      <c r="N84" s="3"/>
+      <c r="O84" s="3"/>
+      <c r="P84" s="3"/>
+      <c r="Q84" s="3"/>
+      <c r="R84" s="3"/>
+      <c r="S84" s="3"/>
+      <c r="T84" s="3">
+        <v>2</v>
+      </c>
+      <c r="U84" s="3"/>
+      <c r="V84" s="3"/>
+      <c r="W84" s="3"/>
+      <c r="X84" s="3"/>
+      <c r="Y84" s="3"/>
+      <c r="Z84" s="3"/>
+      <c r="AA84" s="3"/>
+    </row>
+    <row r="85" spans="2:27">
+      <c r="B85" s="3">
+        <v>2335</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D85" s="4">
+        <v>41963.4216666667</v>
+      </c>
+      <c r="E85" s="5">
+        <v>3</v>
+      </c>
+      <c r="F85" s="3">
+        <v>1</v>
+      </c>
+      <c r="G85" s="5">
+        <v>3</v>
+      </c>
+      <c r="H85" s="5">
+        <v>5</v>
+      </c>
+      <c r="I85" s="3"/>
+      <c r="J85" s="3"/>
+      <c r="K85" s="3"/>
+      <c r="L85" s="3">
+        <v>1</v>
+      </c>
+      <c r="M85" s="3"/>
+      <c r="N85" s="3"/>
+      <c r="O85" s="3"/>
+      <c r="P85" s="3"/>
+      <c r="Q85" s="3"/>
+      <c r="R85" s="3"/>
+      <c r="S85" s="3"/>
+      <c r="T85" s="3"/>
+      <c r="U85" s="3">
+        <v>1</v>
+      </c>
+      <c r="V85" s="3"/>
+      <c r="W85" s="3"/>
+      <c r="X85" s="3"/>
+      <c r="Y85" s="3"/>
+      <c r="Z85" s="3"/>
+      <c r="AA85" s="3"/>
+    </row>
+    <row r="86" spans="2:27">
+      <c r="B86" s="3">
+        <v>2336</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D86" s="4">
+        <v>41963.4217592593</v>
+      </c>
+      <c r="E86" s="5">
+        <v>3</v>
+      </c>
+      <c r="F86" s="3">
+        <v>1</v>
+      </c>
+      <c r="G86" s="5">
+        <v>3</v>
+      </c>
+      <c r="H86" s="5">
+        <v>3</v>
+      </c>
+      <c r="I86" s="3"/>
+      <c r="J86" s="3">
+        <v>3</v>
+      </c>
+      <c r="K86" s="3"/>
+      <c r="L86" s="3"/>
+      <c r="M86" s="3"/>
+      <c r="N86" s="3"/>
+      <c r="O86" s="3"/>
+      <c r="P86" s="3"/>
+      <c r="Q86" s="3"/>
+      <c r="R86" s="3"/>
+      <c r="S86" s="3"/>
+      <c r="T86" s="3"/>
+      <c r="U86" s="3"/>
+      <c r="V86" s="3"/>
+      <c r="W86" s="3"/>
+      <c r="X86" s="3"/>
+      <c r="Y86" s="3"/>
+      <c r="Z86" s="3"/>
+      <c r="AA86" s="3"/>
+    </row>
+    <row r="87" spans="2:27">
+      <c r="B87" s="3">
+        <v>2337</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D87" s="4">
+        <v>41963.4218518519</v>
+      </c>
+      <c r="E87" s="5">
+        <v>3</v>
+      </c>
+      <c r="F87" s="3">
+        <v>1</v>
+      </c>
+      <c r="G87" s="5">
+        <v>3</v>
+      </c>
+      <c r="H87" s="5">
+        <v>3</v>
+      </c>
+      <c r="I87" s="3"/>
+      <c r="J87" s="3">
+        <v>1</v>
+      </c>
+      <c r="K87" s="3">
+        <v>1</v>
+      </c>
+      <c r="L87" s="3"/>
+      <c r="M87" s="3"/>
+      <c r="N87" s="3"/>
+      <c r="O87" s="3"/>
+      <c r="P87" s="3"/>
+      <c r="Q87" s="3"/>
+      <c r="R87" s="3"/>
+      <c r="S87" s="3"/>
+      <c r="T87" s="3"/>
+      <c r="U87" s="3"/>
+      <c r="V87" s="3"/>
+      <c r="W87" s="3"/>
+      <c r="X87" s="3"/>
+      <c r="Y87" s="3"/>
+      <c r="Z87" s="3"/>
+      <c r="AA87" s="3"/>
+    </row>
+    <row r="88" spans="2:27">
+      <c r="B88" s="3">
+        <v>2338</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D88" s="4">
+        <v>41963.4219675926</v>
+      </c>
+      <c r="E88" s="5">
+        <v>3</v>
+      </c>
+      <c r="F88" s="3">
+        <v>1</v>
+      </c>
+      <c r="G88" s="5">
+        <v>3</v>
+      </c>
+      <c r="H88" s="5">
+        <v>3</v>
+      </c>
+      <c r="I88" s="3">
+        <v>2</v>
+      </c>
+      <c r="J88" s="3">
+        <v>2</v>
+      </c>
+      <c r="K88" s="3"/>
+      <c r="L88" s="3"/>
+      <c r="M88" s="3"/>
+      <c r="N88" s="3"/>
+      <c r="O88" s="3"/>
+      <c r="P88" s="3"/>
+      <c r="Q88" s="3"/>
+      <c r="R88" s="3"/>
+      <c r="S88" s="3"/>
+      <c r="T88" s="3"/>
+      <c r="U88" s="3"/>
+      <c r="V88" s="3"/>
+      <c r="W88" s="3"/>
+      <c r="X88" s="3"/>
+      <c r="Y88" s="3"/>
+      <c r="Z88" s="3"/>
+      <c r="AA88" s="3"/>
+    </row>
+    <row r="89" spans="2:27">
+      <c r="B89" s="3">
+        <v>2339</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D89" s="4">
+        <v>41963.4220601852</v>
+      </c>
+      <c r="E89" s="5">
+        <v>3</v>
+      </c>
+      <c r="F89" s="3">
+        <v>1</v>
+      </c>
+      <c r="G89" s="5">
+        <v>3</v>
+      </c>
+      <c r="H89" s="5">
+        <v>3</v>
+      </c>
+      <c r="I89" s="3">
+        <v>2</v>
+      </c>
+      <c r="J89" s="3"/>
+      <c r="K89" s="3">
+        <v>1</v>
+      </c>
+      <c r="L89" s="3"/>
+      <c r="M89" s="3"/>
+      <c r="N89" s="3"/>
+      <c r="O89" s="3"/>
+      <c r="P89" s="3"/>
+      <c r="Q89" s="3"/>
+      <c r="R89" s="3"/>
+      <c r="S89" s="3"/>
+      <c r="T89" s="3"/>
+      <c r="U89" s="3"/>
+      <c r="V89" s="3"/>
+      <c r="W89" s="3"/>
+      <c r="X89" s="3"/>
+      <c r="Y89" s="3"/>
+      <c r="Z89" s="3"/>
+      <c r="AA89" s="3"/>
+    </row>
+    <row r="90" spans="2:27">
+      <c r="B90" s="3">
+        <v>2340</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D90" s="4">
+        <v>41963.4221990741</v>
+      </c>
+      <c r="E90" s="5">
+        <v>3</v>
+      </c>
+      <c r="F90" s="3">
+        <v>1</v>
+      </c>
+      <c r="G90" s="5">
+        <v>3</v>
+      </c>
+      <c r="H90" s="5">
+        <v>3</v>
+      </c>
+      <c r="I90" s="3">
+        <v>4</v>
+      </c>
+      <c r="J90" s="3">
+        <v>1</v>
+      </c>
+      <c r="K90" s="3"/>
+      <c r="L90" s="3"/>
+      <c r="M90" s="3"/>
+      <c r="N90" s="3"/>
+      <c r="O90" s="3"/>
+      <c r="P90" s="3"/>
+      <c r="Q90" s="3"/>
+      <c r="R90" s="3"/>
+      <c r="S90" s="3"/>
+      <c r="T90" s="3"/>
+      <c r="U90" s="3"/>
+      <c r="V90" s="3"/>
+      <c r="W90" s="3"/>
+      <c r="X90" s="3"/>
+      <c r="Y90" s="3"/>
+      <c r="Z90" s="3"/>
+      <c r="AA90" s="3"/>
+    </row>
+    <row r="91" spans="2:27">
+      <c r="B91" s="3">
+        <v>2341</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D91" s="4">
+        <v>41963.4224074074</v>
+      </c>
+      <c r="E91" s="5">
+        <v>3</v>
+      </c>
+      <c r="F91" s="3">
+        <v>1</v>
+      </c>
+      <c r="G91" s="5">
+        <v>3</v>
+      </c>
+      <c r="H91" s="5">
+        <v>3</v>
+      </c>
+      <c r="I91" s="3">
+        <v>6</v>
+      </c>
+      <c r="J91" s="3"/>
+      <c r="K91" s="3"/>
+      <c r="L91" s="3"/>
+      <c r="M91" s="3"/>
+      <c r="N91" s="3"/>
+      <c r="O91" s="3"/>
+      <c r="P91" s="3"/>
+      <c r="Q91" s="3"/>
+      <c r="R91" s="3"/>
+      <c r="S91" s="3"/>
+      <c r="T91" s="3"/>
+      <c r="U91" s="3"/>
+      <c r="V91" s="3"/>
+      <c r="W91" s="3"/>
+      <c r="X91" s="3"/>
+      <c r="Y91" s="3"/>
+      <c r="Z91" s="3"/>
+      <c r="AA91" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>